<commit_message>
Added gov jobs board
</commit_message>
<xml_diff>
--- a/public/route.xlsx
+++ b/public/route.xlsx
@@ -24,171 +24,12 @@
     <t>DIPLOMACY &amp; ANMC N</t>
   </si>
   <si>
-    <t>AMBASSADOR &amp; TUDOR CTR WNW</t>
-  </si>
-  <si>
-    <t>AMBASSADOR &amp; ELMORE ENE</t>
-  </si>
-  <si>
-    <t>ELMORE &amp; SHARON GAGNON SSE</t>
-  </si>
-  <si>
-    <t>ELMORE &amp; PROVIDENCE SSE</t>
-  </si>
-  <si>
-    <t>PROVIDENCE &amp; ALUMNI WNW</t>
-  </si>
-  <si>
     <t>UAA DRIVE &amp; PROVIDENCE NNE</t>
   </si>
   <si>
-    <t>NORTHERN LIGHTS &amp; UAA DR ESE</t>
-  </si>
-  <si>
-    <t>NORTHERN LIGHTS &amp; ARCA DR ESE</t>
-  </si>
-  <si>
-    <t>BRAGAW &amp; NORTHERN LIGHTS NNE</t>
-  </si>
-  <si>
-    <t>BRAGAW &amp; 20TH AVENUE NNE</t>
-  </si>
-  <si>
-    <t>BRAGAW &amp; 16TH AVENUE NNE</t>
-  </si>
-  <si>
-    <t>DEBARR &amp; BRAGAW WNW</t>
-  </si>
-  <si>
-    <t>NORTHWAY &amp; SAN JERONIMO SSE</t>
-  </si>
-  <si>
     <t>NORTHWAY &amp; 801 NORTHWAY EAST</t>
   </si>
   <si>
-    <t>NORTHWAY &amp; PENLAND SSE</t>
-  </si>
-  <si>
-    <t>7TH AVENUE &amp; BRAGAW ESE</t>
-  </si>
-  <si>
-    <t>7TH AVENUE &amp; KLEVIN WSW</t>
-  </si>
-  <si>
-    <t>8TH AVENUE &amp; KLEVIN ESE</t>
-  </si>
-  <si>
-    <t>HOYT &amp; 8TH AVENUE NNE</t>
-  </si>
-  <si>
-    <t>HOYT &amp; 6TH AVENUE SSE</t>
-  </si>
-  <si>
-    <t>HOYT &amp; 4TH AVENUE SSE</t>
-  </si>
-  <si>
-    <t>4TH AVENUE &amp; SHAW WSW</t>
-  </si>
-  <si>
-    <t>4TH AVENUE &amp; PINE WSW</t>
-  </si>
-  <si>
-    <t>PINE &amp; KENAI NNE</t>
-  </si>
-  <si>
-    <t>MCCARREY &amp; CHENA NNE</t>
-  </si>
-  <si>
-    <t>MOUTAIN VIEW &amp; PINE WNW</t>
-  </si>
-  <si>
-    <t>LANE &amp; MOUNTAIN VIEW NNE</t>
-  </si>
-  <si>
-    <t>LANE &amp; THOMPSON NNE</t>
-  </si>
-  <si>
-    <t>PARSONS &amp; LANE WNW</t>
-  </si>
-  <si>
-    <t>PARSONS &amp; KLEVIN NORTH ENE</t>
-  </si>
-  <si>
-    <t>PARSONS &amp; FLOWER NORTH WNW</t>
-  </si>
-  <si>
-    <t>BRAGAW &amp; PARSONS SSW</t>
-  </si>
-  <si>
-    <t>BRAGAW &amp; THOMPSON SSW</t>
-  </si>
-  <si>
-    <t>BRAGAW &amp; PETERKIN SSW</t>
-  </si>
-  <si>
-    <t>MOUTAIN VIEW &amp; BRAGAW WNW</t>
-  </si>
-  <si>
-    <t>MOUTAIN VIEW &amp; PRICE WNW</t>
-  </si>
-  <si>
-    <t>COMMERCIAL &amp; TAYLOR WNW</t>
-  </si>
-  <si>
-    <t>COMMERCIAL &amp; MEYER WNW</t>
-  </si>
-  <si>
-    <t>COMMERCIAL &amp; VIKING WNW</t>
-  </si>
-  <si>
-    <t>COMMERCIAL &amp; INDUSTRIAL NNW</t>
-  </si>
-  <si>
-    <t>COMMERCIAL &amp; CHIPPERFIELD ENE</t>
-  </si>
-  <si>
-    <t>3RD AVENUE &amp; REEVE WNW</t>
-  </si>
-  <si>
-    <t>3RD AVENUE &amp; UNGA WNW</t>
-  </si>
-  <si>
-    <t>3RD AVENUE &amp; SITKA WNW</t>
-  </si>
-  <si>
-    <t>3RD AVENUE &amp; CONCRETE ENE</t>
-  </si>
-  <si>
-    <t>3RD AVENUE &amp; ORCA WNW</t>
-  </si>
-  <si>
-    <t>3RD AVENUE &amp; POST ROAD WNW</t>
-  </si>
-  <si>
-    <t>3RD AVENUE &amp; KARLUK WNW</t>
-  </si>
-  <si>
-    <t>3RD AVENUE &amp; GAMBELL WNW</t>
-  </si>
-  <si>
-    <t>3RD AVENUE &amp; EAGLE WNW</t>
-  </si>
-  <si>
-    <t>3RD AVENUE &amp; CORDOVA ENE</t>
-  </si>
-  <si>
-    <t>3RD AVENUE &amp; BARROW WNW</t>
-  </si>
-  <si>
-    <t>C STREET &amp; 5TH AVENUE NNW</t>
-  </si>
-  <si>
-    <t>C STREET &amp; 7TH AVENUE SSW</t>
-  </si>
-  <si>
-    <t>9TH AVENUE &amp; C STREET WNW</t>
-  </si>
-  <si>
     <t>9TH AVENUE &amp; F STREET WNW</t>
   </si>
   <si>
@@ -199,6 +40,165 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>AMBASSADOR &amp; TUDOR CENTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMBASSADOR &amp; ELMORE </t>
+  </si>
+  <si>
+    <t>ELMORE &amp; SHARON GAGNON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELMORE &amp; PROVIDENCE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROVIDENCE &amp; ALUMNI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9TH AVENUE &amp; C STREET </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C STREET &amp; 7TH AVENUE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C STREET &amp; 5TH AVENUE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3RD AVENUE &amp; BARROW </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3RD AVENUE &amp; CORDOVA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3RD AVENUE &amp; EAGLE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3RD AVENUE &amp; GAMBELL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3RD AVENUE &amp; KARLUK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3RD AVENUE &amp; POST ROAD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRAGAW &amp; THOMPSON </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRAGAW &amp; PARSONS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARSONS &amp; FLOWER NORTH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARSONS &amp; KLEVIN NORTH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRAGAW &amp; 16TH AVENUE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NORTHERN LIGHTS &amp; UAA DR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NORTHERN LIGHTS &amp; ARCA DR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7TH AVENUE &amp; BRAGAW </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7TH AVENUE &amp; KLEVIN </t>
+  </si>
+  <si>
+    <t>4TH AVENUE &amp; SHAW </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4TH AVENUE &amp; PINE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCCARREY &amp; CHENA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOUTAIN VIEW &amp; PINE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LANE &amp; MOUNTAIN VIEW </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARSONS &amp; LANE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LANE &amp; THOMPSON </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOYT ST &amp; 8TH AVENUE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOYT ST &amp; 4TH AVENUE </t>
+  </si>
+  <si>
+    <t>PINE ST &amp; KENAI AVE</t>
+  </si>
+  <si>
+    <t>N BRAGAW ST &amp; PETERKIN AVE</t>
+  </si>
+  <si>
+    <t>MOUTAIN VIEW &amp; N BRAGAW ST</t>
+  </si>
+  <si>
+    <t>MOUNTAIN VIEW DR &amp; PRICE ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMMERCIAL DRIVE &amp; VIKING DRIVE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMMERCIAL DRIVE &amp; MEYER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMMERCIAL DRIVE &amp; TAYLOR </t>
+  </si>
+  <si>
+    <t>COMMERCIAL DRIVE &amp; CHIPPERFIELD DRIVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMMERCIAL DRIVE &amp; INDUSTRIAL WAY </t>
+  </si>
+  <si>
+    <t>COMMERCIAL DRIVE &amp; REEVE BLVD</t>
+  </si>
+  <si>
+    <t>E 3RD AVENUE &amp; UNGA ST</t>
+  </si>
+  <si>
+    <t>E 3RD AVENUE &amp; SITKA ST</t>
+  </si>
+  <si>
+    <t>E 3RD AVENUE &amp; CONCRETE ST</t>
+  </si>
+  <si>
+    <t>E 3RD AVENUE &amp; ORCA ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRAGAW ST &amp; E 20TH AVENUE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRAGAW ST &amp; NORTHERN LIGHTS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEBARR ROAD &amp; BRAGAW ST  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NORTHWAY DRIVE &amp; SAN JERONIMO DRIVE </t>
+  </si>
+  <si>
+    <t>NORTHWAY DRIVE &amp; PENLAND PARKWAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E 8TH AVENUE &amp; KLEVIN ST </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOYT ST &amp; E 6TH AVENUE </t>
   </si>
 </sst>
 </file>
@@ -1511,10 +1511,10 @@
   <dimension ref="A1:IQ59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1:F1048576"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -1524,10 +1524,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="20.5" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" customHeight="1">
@@ -1543,7 +1543,7 @@
         <v>3009</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" customHeight="1">
@@ -1551,7 +1551,7 @@
         <v>3007</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="44" customHeight="1">
@@ -1559,7 +1559,7 @@
         <v>3013</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="44" customHeight="1">
@@ -1567,7 +1567,7 @@
         <v>611</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" customHeight="1">
@@ -1575,7 +1575,7 @@
         <v>1223</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="44" customHeight="1">
@@ -1583,7 +1583,7 @@
         <v>293</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="44" customHeight="1">
@@ -1591,7 +1591,7 @@
         <v>1312</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="44" customHeight="1">
@@ -1599,7 +1599,7 @@
         <v>1313</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="44" customHeight="1">
@@ -1607,7 +1607,7 @@
         <v>1314</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="44" customHeight="1">
@@ -1615,7 +1615,7 @@
         <v>1315</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="44" customHeight="1">
@@ -1623,7 +1623,7 @@
         <v>1316</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" customHeight="1">
@@ -1631,7 +1631,7 @@
         <v>1317</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="44" customHeight="1">
@@ -1639,7 +1639,7 @@
         <v>1318</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="44" customHeight="1">
@@ -1647,7 +1647,7 @@
         <v>1319</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" customHeight="1">
@@ -1655,7 +1655,7 @@
         <v>1320</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" customHeight="1">
@@ -1663,7 +1663,7 @@
         <v>748</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" customHeight="1">
@@ -1671,7 +1671,7 @@
         <v>749</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30" customHeight="1">
@@ -1679,7 +1679,7 @@
         <v>1324</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" customHeight="1">
@@ -1687,7 +1687,7 @@
         <v>1325</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30" customHeight="1">
@@ -1695,7 +1695,7 @@
         <v>1326</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30" customHeight="1">
@@ -1703,7 +1703,7 @@
         <v>1327</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="30" customHeight="1">
@@ -1711,7 +1711,7 @@
         <v>754</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" customHeight="1">
@@ -1719,7 +1719,7 @@
         <v>755</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30" customHeight="1">
@@ -1727,7 +1727,7 @@
         <v>1330</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="30" customHeight="1">
@@ -1735,7 +1735,7 @@
         <v>1331</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="30" customHeight="1">
@@ -1743,7 +1743,7 @@
         <v>1332</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="44" customHeight="1">
@@ -1751,7 +1751,7 @@
         <v>1333</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="44" customHeight="1">
@@ -1759,7 +1759,7 @@
         <v>1334</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="30" customHeight="1">
@@ -1767,7 +1767,7 @@
         <v>1335</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="44" customHeight="1">
@@ -1775,7 +1775,7 @@
         <v>1336</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="44" customHeight="1">
@@ -1783,7 +1783,7 @@
         <v>1337</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="30" customHeight="1">
@@ -1791,7 +1791,7 @@
         <v>1338</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="44" customHeight="1">
@@ -1799,7 +1799,7 @@
         <v>1339</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="30" customHeight="1">
@@ -1807,7 +1807,7 @@
         <v>1340</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="44" customHeight="1">
@@ -1815,7 +1815,7 @@
         <v>1341</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="30" customHeight="1">
@@ -1823,7 +1823,7 @@
         <v>1342</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="30" customHeight="1">
@@ -1831,7 +1831,7 @@
         <v>1343</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="30" customHeight="1">
@@ -1839,7 +1839,7 @@
         <v>1344</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="30" customHeight="1">
@@ -1847,7 +1847,7 @@
         <v>1345</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="44" customHeight="1">
@@ -1855,7 +1855,7 @@
         <v>1346</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="44" customHeight="1">
@@ -1863,7 +1863,7 @@
         <v>1347</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="30" customHeight="1">
@@ -1871,7 +1871,7 @@
         <v>3018</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="30" customHeight="1">
@@ -1879,7 +1879,7 @@
         <v>1348</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="30" customHeight="1">
@@ -1887,7 +1887,7 @@
         <v>3689</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="44" customHeight="1">
@@ -1895,7 +1895,7 @@
         <v>1349</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="30" customHeight="1">
@@ -1903,7 +1903,7 @@
         <v>1350</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="44" customHeight="1">
@@ -1911,7 +1911,7 @@
         <v>1351</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="30" customHeight="1">
@@ -1919,7 +1919,7 @@
         <v>1352</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="30" customHeight="1">
@@ -1927,7 +1927,7 @@
         <v>1353</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="30" customHeight="1">
@@ -1935,7 +1935,7 @@
         <v>1354</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="30" customHeight="1">
@@ -1943,7 +1943,7 @@
         <v>1355</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="30" customHeight="1">
@@ -1951,7 +1951,7 @@
         <v>1356</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="44" customHeight="1">
@@ -1959,7 +1959,7 @@
         <v>1357</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="44" customHeight="1">
@@ -1967,7 +1967,7 @@
         <v>3</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="44" customHeight="1">
@@ -1975,7 +1975,7 @@
         <v>652</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="30" customHeight="1">
@@ -1983,7 +1983,7 @@
         <v>3527</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="30" customHeight="1">
@@ -1991,7 +1991,7 @@
         <v>2051</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>